<commit_message>
Added Software Design Document
</commit_message>
<xml_diff>
--- a/Responsibility Assignment Matrix.xlsx
+++ b/Responsibility Assignment Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenurquhart/Desktop/Tri 2 2023/2810ICT Software Technologies /2810ICT-7810ICT-2023-Assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1496638-A78B-9044-B212-673DB79B8F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E7B2AF6-EFC0-5A4A-BC6D-0CA74ECEAB9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{4B5AE6D9-5A5F-B940-A879-54F099FA52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>Responsibility Assignment Matrix (RAM)</t>
   </si>
@@ -81,6 +81,36 @@
   </si>
   <si>
     <t>Work Breakdown Structure</t>
+  </si>
+  <si>
+    <t>1.1 Problem Background</t>
+  </si>
+  <si>
+    <t>1.2 System Overview</t>
+  </si>
+  <si>
+    <t>1.3 Potential Benefits</t>
+  </si>
+  <si>
+    <t>2.1 User Requirements</t>
+  </si>
+  <si>
+    <t>2.2 Software Requirements</t>
+  </si>
+  <si>
+    <t>2.3 Use Cases</t>
+  </si>
+  <si>
+    <t>3.1 Software Design</t>
+  </si>
+  <si>
+    <t>3.2 System Componenets</t>
+  </si>
+  <si>
+    <t>4.1 Structural Design</t>
+  </si>
+  <si>
+    <t>4.2 Visual Design</t>
   </si>
 </sst>
 </file>
@@ -260,7 +290,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -272,21 +302,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -311,6 +331,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -629,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E563F16A-F496-4941-8E32-8588839456FC}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -641,14 +670,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -656,222 +685,292 @@
       </c>
     </row>
     <row r="3" spans="1:6" s="2" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="11"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="17" t="s">
+      <c r="B5" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D6" s="19" t="s">
+      <c r="B6" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="15" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="19" t="s">
+      <c r="B8" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="17"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="13"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
+      <c r="A10" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="17"/>
+      <c r="A11" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-      <c r="D12" s="19"/>
+      <c r="A12" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="7"/>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="17"/>
+      <c r="A13" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="19"/>
+      <c r="A14" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="7"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="20"/>
-      <c r="D15" s="17"/>
+      <c r="A15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
+      <c r="A16" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="20"/>
-      <c r="C17" s="20"/>
-      <c r="D17" s="17"/>
+      <c r="A17" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
+      <c r="A18" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="7"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="17"/>
+      <c r="A19" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="19"/>
+      <c r="A20" s="11"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="15"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="7"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="17"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="13"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="19"/>
+      <c r="A22" s="11"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="14"/>
+      <c r="D22" s="15"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="7"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="20"/>
-      <c r="D23" s="17"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="13"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="19"/>
+      <c r="A24" s="11"/>
+      <c r="B24" s="14"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="15"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="7"/>
-      <c r="B25" s="20"/>
-      <c r="C25" s="20"/>
-      <c r="D25" s="17"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="16"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="13"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="7"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="17"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="16"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="13"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="7"/>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="17"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="16"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="13"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="7"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="17"/>
+      <c r="A28" s="6"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="13"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="7"/>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="17"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="16"/>
+      <c r="C29" s="16"/>
+      <c r="D29" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Responsibility Assignment Matrix.xlsx
</commit_message>
<xml_diff>
--- a/Responsibility Assignment Matrix.xlsx
+++ b/Responsibility Assignment Matrix.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenurquhart/Desktop/Tri 2 2023/2810ICT Software Technologies /2810ICT-7810ICT-2023-Assignment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenurquhart/Desktop/Tri 2 2023/2810ICT Software Technologies /Part B - Working Copy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01444521-CF16-A14F-8D37-70FC75426585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82B3BE90-07E7-BE46-94B4-72ABC594748B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="18380" xr2:uid="{4B5AE6D9-5A5F-B940-A879-54F099FA52D6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="50">
   <si>
     <t>Person</t>
   </si>
@@ -123,13 +123,76 @@
   </si>
   <si>
     <t>R C I</t>
+  </si>
+  <si>
+    <t>Python Application</t>
+  </si>
+  <si>
+    <t>Software Testing Report.docx</t>
+  </si>
+  <si>
+    <t>User Manual.docx</t>
+  </si>
+  <si>
+    <t>Executive Summary.docx</t>
+  </si>
+  <si>
+    <t>Project Plan.docx Part B Update</t>
+  </si>
+  <si>
+    <t>Updated Gantt Chart.xlsx</t>
+  </si>
+  <si>
+    <t>Coding</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Images</t>
+  </si>
+  <si>
+    <t>Testing Data</t>
+  </si>
+  <si>
+    <t>WBS Updates</t>
+  </si>
+  <si>
+    <t>Activity Definitions Updates</t>
+  </si>
+  <si>
+    <t>Estimations Updates</t>
+  </si>
+  <si>
+    <t>Function Testing</t>
+  </si>
+  <si>
+    <t>Visualisation Testing</t>
+  </si>
+  <si>
+    <t>Reporting</t>
+  </si>
+  <si>
+    <t>File Content</t>
+  </si>
+  <si>
+    <t>Responsiblility Assignment Matrix - Part B</t>
+  </si>
+  <si>
+    <t>Progress Tracking</t>
+  </si>
+  <si>
+    <t>R A C I</t>
+  </si>
+  <si>
+    <t>R A C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -184,6 +247,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -199,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -482,11 +553,68 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -497,19 +625,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
@@ -517,53 +637,100 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -880,10 +1047,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E563F16A-F496-4941-8E32-8588839456FC}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -891,58 +1058,94 @@
     <col min="1" max="1" width="28.5" customWidth="1"/>
     <col min="2" max="3" width="7" customWidth="1"/>
     <col min="4" max="4" width="7.1640625" customWidth="1"/>
+    <col min="6" max="6" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-    </row>
-    <row r="2" spans="1:4" s="19" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="F1" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+    </row>
+    <row r="2" spans="1:9" s="13" customFormat="1" ht="12" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="F2" s="13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="10"/>
-    </row>
-    <row r="4" spans="1:4" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
+      <c r="C3" s="28"/>
+      <c r="D3" s="29"/>
+      <c r="F3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="27" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="28"/>
+      <c r="I3" s="29"/>
+    </row>
+    <row r="4" spans="1:9" s="1" customFormat="1" ht="20" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="21" t="s">
+      <c r="C4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="19" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
+      <c r="F4" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="6" customFormat="1" ht="19" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="24"/>
-      <c r="D5" s="25"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="B5" s="17"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="19"/>
+      <c r="F5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="39"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="19"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -951,12 +1154,24 @@
       <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="11" t="s">
+      <c r="F6" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="26" t="s">
+      <c r="B7" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -965,12 +1180,24 @@
       <c r="D7" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="11" t="s">
+      <c r="F7" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -979,12 +1206,16 @@
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="11" t="s">
+      <c r="F8" s="32"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="26" t="s">
+      <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -993,12 +1224,18 @@
       <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="F9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G9" s="41"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="42"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="26" t="s">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1007,26 +1244,54 @@
       <c r="D10" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
-      <c r="B11" s="26"/>
+      <c r="F10" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="7"/>
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="F11" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="11" t="s">
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="43"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="44"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1035,12 +1300,18 @@
       <c r="D13" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="F13" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="41"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="42"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1049,12 +1320,24 @@
       <c r="D14" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="11" t="s">
+      <c r="F14" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="G14" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1063,12 +1346,24 @@
       <c r="D15" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="11" t="s">
+      <c r="F15" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1077,12 +1372,24 @@
       <c r="D16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
+      <c r="F16" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="26" t="s">
+      <c r="B17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1091,12 +1398,16 @@
       <c r="D17" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="11" t="s">
+      <c r="F17" s="32"/>
+      <c r="G17" s="40"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="2"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1105,12 +1416,18 @@
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="11" t="s">
+      <c r="F18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" s="41"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="42"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1119,12 +1436,24 @@
       <c r="D19" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="F19" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1133,12 +1462,24 @@
       <c r="D20" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="11" t="s">
+      <c r="F20" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="G20" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1147,91 +1488,185 @@
       <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="F21" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" s="32" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="6"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A33" s="4"/>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="B22" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="32"/>
+      <c r="G22" s="40"/>
+      <c r="H22" s="3"/>
+      <c r="I22" s="2"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+      <c r="F23" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="G23" s="41"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="42"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+      <c r="F24" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="F25" s="31" t="s">
+        <v>43</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="F26" s="31" t="s">
+        <v>44</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="F27" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="G27" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="F28" s="7"/>
+      <c r="G28" s="40"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="2"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="F29" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="G29" s="41"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="42"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="F30" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>9</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="F31" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>9</v>
+      </c>
+      <c r="H31" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="F32" s="30"/>
+    </row>
+    <row r="33" spans="6:6" x14ac:dyDescent="0.2">
+      <c r="F33" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="G3:I3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>